<commit_message>
Add search and fixed header
</commit_message>
<xml_diff>
--- a/STANFORD/AGREGATOR/stanford_daily_report.xlsx
+++ b/STANFORD/AGREGATOR/stanford_daily_report.xlsx
@@ -43,6 +43,9 @@
     <t>Total</t>
   </si>
   <si>
+    <t>Jun-2017</t>
+  </si>
+  <si>
     <t>May-2017</t>
   </si>
   <si>
@@ -74,9 +77,6 @@
   </si>
   <si>
     <t>Jul-2016</t>
-  </si>
-  <si>
-    <t>Jun-2016</t>
   </si>
   <si>
     <t>SearchWorks</t>
@@ -1422,20 +1422,20 @@
         <v>91</v>
       </c>
       <c r="J4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="5">
         <v>1</v>
       </c>
       <c r="L4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
         <v>2</v>
       </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
       <c r="O4" s="5">
         <v>0</v>
       </c>
@@ -1443,19 +1443,19 @@
         <v>0</v>
       </c>
       <c r="Q4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="5">
         <v>1</v>
       </c>
       <c r="U4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="5" customFormat="1">
@@ -1487,37 +1487,37 @@
         <v>104</v>
       </c>
       <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
         <v>2</v>
       </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
       <c r="L5" s="5">
         <v>0</v>
       </c>
       <c r="M5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="5">
         <v>1</v>
       </c>
       <c r="Q5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="5">
         <v>1</v>
       </c>
       <c r="T5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="5">
         <v>0</v>
@@ -1552,25 +1552,25 @@
         <v>116</v>
       </c>
       <c r="J6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="5">
         <v>0</v>
       </c>
       <c r="O6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="5">
         <v>0</v>
@@ -1585,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="U6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="5" customFormat="1">
@@ -1617,19 +1617,19 @@
         <v>55</v>
       </c>
       <c r="J7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="5">
         <v>0</v>
       </c>
       <c r="M7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="5">
         <v>0</v>
@@ -1641,16 +1641,16 @@
         <v>0</v>
       </c>
       <c r="R7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="5" customFormat="1">
@@ -1679,37 +1679,37 @@
         <v>74</v>
       </c>
       <c r="J8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="5">
         <v>0</v>
       </c>
       <c r="M8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" s="5">
         <v>0</v>
       </c>
       <c r="P8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="5">
         <v>0</v>
       </c>
       <c r="S8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="5">
         <v>0</v>
@@ -1744,7 +1744,7 @@
         <v>216</v>
       </c>
       <c r="J9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="5">
         <v>1</v>
@@ -1756,19 +1756,19 @@
         <v>1</v>
       </c>
       <c r="N9" s="5">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5">
         <v>2</v>
       </c>
-      <c r="O9" s="5">
-        <v>0</v>
-      </c>
       <c r="P9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5">
         <v>2</v>
       </c>
-      <c r="Q9" s="5">
-        <v>0</v>
-      </c>
       <c r="R9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" s="5">
         <v>1</v>
@@ -1806,19 +1806,19 @@
         <v>62</v>
       </c>
       <c r="J10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="5">
         <v>1</v>
       </c>
       <c r="L10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="5">
         <v>0</v>
@@ -1871,19 +1871,19 @@
         <v>802</v>
       </c>
       <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
         <v>3</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>5</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>4</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>6</v>
-      </c>
-      <c r="N11" s="2">
-        <v>4</v>
       </c>
       <c r="O11" s="2">
         <v>4</v>
@@ -1898,13 +1898,13 @@
         <v>4</v>
       </c>
       <c r="S11" s="2">
+        <v>4</v>
+      </c>
+      <c r="T11" s="2">
         <v>2</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>4</v>
-      </c>
-      <c r="U11" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="2" customFormat="1">
@@ -1936,37 +1936,37 @@
         <v>77</v>
       </c>
       <c r="J12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
       </c>
       <c r="M12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="2">
         <v>0</v>
       </c>
       <c r="P12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" s="2">
         <v>0</v>
       </c>
       <c r="S12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12" s="2">
         <v>0</v>
@@ -1998,37 +1998,37 @@
         <v>140</v>
       </c>
       <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
         <v>3</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>5</v>
-      </c>
-      <c r="L13" s="2">
-        <v>3</v>
       </c>
       <c r="M13" s="2">
         <v>3</v>
       </c>
       <c r="N13" s="2">
+        <v>3</v>
+      </c>
+      <c r="O13" s="2">
         <v>6</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>3</v>
       </c>
-      <c r="P13" s="2">
+      <c r="Q13" s="2">
         <v>4</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="R13" s="2">
         <v>3</v>
       </c>
-      <c r="R13" s="2">
+      <c r="S13" s="2">
         <v>6</v>
       </c>
-      <c r="S13" s="2">
+      <c r="T13" s="2">
         <v>5</v>
-      </c>
-      <c r="T13" s="2">
-        <v>4</v>
       </c>
       <c r="U13" s="2">
         <v>4</v>
@@ -2060,16 +2060,16 @@
         <v>221</v>
       </c>
       <c r="J14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
         <v>2</v>
       </c>
-      <c r="L14" s="2">
-        <v>0</v>
-      </c>
       <c r="M14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
         <v>1</v>
@@ -2078,13 +2078,13 @@
         <v>1</v>
       </c>
       <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
         <v>2</v>
       </c>
-      <c r="Q14" s="2">
-        <v>0</v>
-      </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>1</v>
@@ -2122,20 +2122,20 @@
         <v>61</v>
       </c>
       <c r="J15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="2">
         <v>0</v>
       </c>
       <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
         <v>2</v>
       </c>
-      <c r="N15" s="2">
-        <v>0</v>
-      </c>
       <c r="O15" s="2">
         <v>0</v>
       </c>
@@ -2149,13 +2149,13 @@
         <v>0</v>
       </c>
       <c r="S15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="2" customFormat="1">
@@ -2187,19 +2187,19 @@
         <v>55</v>
       </c>
       <c r="J16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
       </c>
       <c r="M16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="2">
         <v>0</v>
@@ -2214,10 +2214,10 @@
         <v>0</v>
       </c>
       <c r="S16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" s="2">
         <v>0</v>
@@ -2249,10 +2249,10 @@
         <v>84</v>
       </c>
       <c r="J17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="2">
         <v>0</v>
@@ -2261,25 +2261,25 @@
         <v>0</v>
       </c>
       <c r="N17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="2">
         <v>1</v>
       </c>
       <c r="R17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17" s="2">
         <v>0</v>
       </c>
       <c r="T17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" s="2">
         <v>1</v>
@@ -2314,22 +2314,22 @@
         <v>177</v>
       </c>
       <c r="J18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
       </c>
       <c r="M18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2">
         <v>1</v>
       </c>
       <c r="O18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
@@ -2338,16 +2338,16 @@
         <v>0</v>
       </c>
       <c r="R18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" s="2">
         <v>1</v>
       </c>
       <c r="T18" s="2">
+        <v>1</v>
+      </c>
+      <c r="U18" s="2">
         <v>2</v>
-      </c>
-      <c r="U18" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="2" customFormat="1">
@@ -2379,40 +2379,40 @@
         <v>184</v>
       </c>
       <c r="J19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
         <v>2</v>
       </c>
-      <c r="L19" s="2">
-        <v>1</v>
-      </c>
       <c r="M19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="2">
         <v>1</v>
       </c>
       <c r="R19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="2">
+        <v>0</v>
+      </c>
+      <c r="T19" s="2">
         <v>2</v>
       </c>
-      <c r="T19" s="2">
-        <v>1</v>
-      </c>
       <c r="U19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:21" s="2" customFormat="1">
@@ -2444,10 +2444,10 @@
         <v>53</v>
       </c>
       <c r="J20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
@@ -2462,10 +2462,10 @@
         <v>0</v>
       </c>
       <c r="P20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" s="2">
         <v>0</v>
@@ -2474,10 +2474,10 @@
         <v>0</v>
       </c>
       <c r="T20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="2" customFormat="1">
@@ -2509,40 +2509,40 @@
         <v>390</v>
       </c>
       <c r="J21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
         <v>3</v>
       </c>
-      <c r="L21" s="2">
-        <v>1</v>
-      </c>
       <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2">
         <v>3</v>
-      </c>
-      <c r="N21" s="2">
-        <v>2</v>
       </c>
       <c r="O21" s="2">
         <v>2</v>
       </c>
       <c r="P21" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="2">
         <v>3</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="R21" s="2">
         <v>2</v>
       </c>
-      <c r="R21" s="2">
-        <v>1</v>
-      </c>
       <c r="S21" s="2">
         <v>1</v>
       </c>
       <c r="T21" s="2">
+        <v>1</v>
+      </c>
+      <c r="U21" s="2">
         <v>2</v>
-      </c>
-      <c r="U21" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="2" customFormat="1">
@@ -2571,40 +2571,40 @@
         <v>91</v>
       </c>
       <c r="J22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" s="2">
         <v>0</v>
       </c>
       <c r="U22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="2" customFormat="1">
@@ -2633,28 +2633,28 @@
         <v>50</v>
       </c>
       <c r="J23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="2">
         <v>0</v>
       </c>
       <c r="M23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" s="2">
         <v>0</v>
       </c>
       <c r="P23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" s="2">
         <v>0</v>
@@ -2663,10 +2663,10 @@
         <v>0</v>
       </c>
       <c r="T23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="2" customFormat="1">
@@ -2698,16 +2698,16 @@
         <v>193</v>
       </c>
       <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
         <v>2</v>
       </c>
-      <c r="K24" s="2">
-        <v>1</v>
-      </c>
       <c r="L24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" s="2">
         <v>1</v>
@@ -2716,22 +2716,22 @@
         <v>1</v>
       </c>
       <c r="P24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="2">
+        <v>0</v>
+      </c>
+      <c r="R24" s="2">
         <v>2</v>
       </c>
-      <c r="R24" s="2">
-        <v>0</v>
-      </c>
       <c r="S24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T24" s="2">
+        <v>1</v>
+      </c>
+      <c r="U24" s="2">
         <v>3</v>
-      </c>
-      <c r="U24" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:21" s="2" customFormat="1">
@@ -2763,19 +2763,19 @@
         <v>67</v>
       </c>
       <c r="J25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="2">
         <v>0</v>
       </c>
       <c r="M25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="2">
         <v>0</v>
@@ -2784,10 +2784,10 @@
         <v>0</v>
       </c>
       <c r="Q25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" s="2">
         <v>0</v>
@@ -2828,22 +2828,22 @@
         <v>71</v>
       </c>
       <c r="J26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="2">
         <v>1</v>
       </c>
       <c r="L26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="2">
         <v>0</v>
       </c>
       <c r="N26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="2">
         <v>0</v>
@@ -2852,10 +2852,10 @@
         <v>0</v>
       </c>
       <c r="R26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="2">
         <v>0</v>
@@ -2893,16 +2893,16 @@
         <v>91</v>
       </c>
       <c r="J27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="2">
         <v>0</v>
@@ -2917,10 +2917,10 @@
         <v>0</v>
       </c>
       <c r="R27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T27" s="2">
         <v>0</v>
@@ -2958,34 +2958,34 @@
         <v>0</v>
       </c>
       <c r="K28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="2">
         <v>0</v>
       </c>
       <c r="N28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="2">
         <v>0</v>
       </c>
       <c r="S28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28" s="2">
         <v>0</v>
@@ -3023,16 +3023,16 @@
         <v>0</v>
       </c>
       <c r="K29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="2">
         <v>0</v>
@@ -3041,16 +3041,16 @@
         <v>0</v>
       </c>
       <c r="Q29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S29" s="2">
         <v>0</v>
       </c>
       <c r="T29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U29" s="2">
         <v>1</v>
@@ -3088,37 +3088,37 @@
         <v>0</v>
       </c>
       <c r="K30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="2">
         <v>1</v>
       </c>
       <c r="M30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R30" s="2">
         <v>0</v>
       </c>
       <c r="S30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:21" s="2" customFormat="1">
@@ -3153,10 +3153,10 @@
         <v>0</v>
       </c>
       <c r="K31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="2">
         <v>0</v>
@@ -3171,10 +3171,10 @@
         <v>0</v>
       </c>
       <c r="Q31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S31" s="2">
         <v>0</v>
@@ -3218,13 +3218,13 @@
         <v>0</v>
       </c>
       <c r="K32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32" s="2">
         <v>1</v>
@@ -3233,7 +3233,7 @@
         <v>1</v>
       </c>
       <c r="P32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="2">
         <v>0</v>
@@ -3245,10 +3245,10 @@
         <v>0</v>
       </c>
       <c r="T32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:21" s="2" customFormat="1">
@@ -3283,28 +3283,28 @@
         <v>0</v>
       </c>
       <c r="K33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="2">
         <v>0</v>
       </c>
       <c r="N33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" s="2">
         <v>0</v>
       </c>
       <c r="Q33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S33" s="2">
         <v>0</v>
@@ -3313,7 +3313,7 @@
         <v>0</v>
       </c>
       <c r="U33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:21" s="2" customFormat="1">
@@ -3348,10 +3348,10 @@
         <v>0</v>
       </c>
       <c r="L34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" s="2">
         <v>0</v>
@@ -3375,7 +3375,7 @@
         <v>0</v>
       </c>
       <c r="U34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:21" s="2" customFormat="1">
@@ -3413,11 +3413,11 @@
         <v>0</v>
       </c>
       <c r="L35" s="2">
+        <v>0</v>
+      </c>
+      <c r="M35" s="2">
         <v>33</v>
       </c>
-      <c r="M35" s="2">
-        <v>0</v>
-      </c>
       <c r="N35" s="2">
         <v>0</v>
       </c>
@@ -3437,10 +3437,10 @@
         <v>0</v>
       </c>
       <c r="T35" s="2">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="U35" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:21" s="2" customFormat="1">
@@ -3478,10 +3478,10 @@
         <v>0</v>
       </c>
       <c r="L36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N36" s="2">
         <v>0</v>
@@ -3502,10 +3502,10 @@
         <v>0</v>
       </c>
       <c r="T36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:21" s="2" customFormat="1">
@@ -3540,10 +3540,10 @@
         <v>0</v>
       </c>
       <c r="L37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N37" s="2">
         <v>0</v>
@@ -3552,22 +3552,22 @@
         <v>0</v>
       </c>
       <c r="P37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" s="2">
         <v>0</v>
       </c>
       <c r="S37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37" s="2">
         <v>1</v>
       </c>
       <c r="U37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:21" s="2" customFormat="1">
@@ -3605,16 +3605,16 @@
         <v>0</v>
       </c>
       <c r="L38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P38" s="2">
         <v>0</v>
@@ -3626,10 +3626,10 @@
         <v>0</v>
       </c>
       <c r="S38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38" s="2">
         <v>0</v>
@@ -3667,10 +3667,10 @@
         <v>0</v>
       </c>
       <c r="L39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39" s="2">
         <v>0</v>
@@ -3691,10 +3691,10 @@
         <v>0</v>
       </c>
       <c r="T39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:21" s="2" customFormat="1">
@@ -3729,10 +3729,10 @@
         <v>0</v>
       </c>
       <c r="L40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N40" s="2">
         <v>0</v>
@@ -3750,13 +3750,13 @@
         <v>0</v>
       </c>
       <c r="S40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:21" s="2" customFormat="1">
@@ -3794,10 +3794,10 @@
         <v>0</v>
       </c>
       <c r="L41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N41" s="2">
         <v>0</v>
@@ -3806,10 +3806,10 @@
         <v>0</v>
       </c>
       <c r="P41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41" s="2">
         <v>0</v>
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="U41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:21" s="2" customFormat="1">
@@ -3856,10 +3856,10 @@
         <v>0</v>
       </c>
       <c r="L42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N42" s="2">
         <v>0</v>
@@ -3871,16 +3871,16 @@
         <v>0</v>
       </c>
       <c r="Q42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S42" s="2">
         <v>0</v>
       </c>
       <c r="T42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U42" s="2">
         <v>1</v>
@@ -3924,10 +3924,10 @@
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O43" s="2">
         <v>0</v>
@@ -3939,10 +3939,10 @@
         <v>0</v>
       </c>
       <c r="R43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T43" s="2">
         <v>0</v>
@@ -3989,10 +3989,10 @@
         <v>0</v>
       </c>
       <c r="M44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" s="2">
         <v>0</v>
@@ -4001,10 +4001,10 @@
         <v>0</v>
       </c>
       <c r="Q44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S44" s="2">
         <v>0</v>
@@ -4048,10 +4048,10 @@
         <v>0</v>
       </c>
       <c r="M45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O45" s="2">
         <v>0</v>
@@ -4066,10 +4066,10 @@
         <v>0</v>
       </c>
       <c r="S45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U45" s="2">
         <v>0</v>
@@ -4113,28 +4113,28 @@
         <v>0</v>
       </c>
       <c r="M46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46" s="2">
         <v>1</v>
       </c>
       <c r="O46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" s="2">
         <v>0</v>
       </c>
       <c r="S46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U46" s="2">
         <v>0</v>
@@ -4178,10 +4178,10 @@
         <v>0</v>
       </c>
       <c r="M47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O47" s="2">
         <v>0</v>
@@ -4190,10 +4190,10 @@
         <v>0</v>
       </c>
       <c r="Q47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S47" s="2">
         <v>0</v>
@@ -4202,7 +4202,7 @@
         <v>0</v>
       </c>
       <c r="U47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:21" s="2" customFormat="1">
@@ -4243,25 +4243,25 @@
         <v>0</v>
       </c>
       <c r="M48" s="2">
+        <v>0</v>
+      </c>
+      <c r="N48" s="2">
         <v>3</v>
       </c>
-      <c r="N48" s="2">
-        <v>0</v>
-      </c>
       <c r="O48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P48" s="2">
         <v>1</v>
       </c>
       <c r="Q48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T48" s="2">
         <v>0</v>
@@ -4311,10 +4311,10 @@
         <v>0</v>
       </c>
       <c r="N49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49" s="2">
         <v>0</v>
@@ -4376,10 +4376,10 @@
         <v>0</v>
       </c>
       <c r="N50" s="2">
+        <v>0</v>
+      </c>
+      <c r="O50" s="2">
         <v>2</v>
-      </c>
-      <c r="O50" s="2">
-        <v>0</v>
       </c>
       <c r="P50" s="2">
         <v>0</v>
@@ -4441,10 +4441,10 @@
         <v>0</v>
       </c>
       <c r="N51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P51" s="2">
         <v>0</v>
@@ -4459,10 +4459,10 @@
         <v>0</v>
       </c>
       <c r="T51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:21" s="2" customFormat="1">
@@ -4509,10 +4509,10 @@
         <v>0</v>
       </c>
       <c r="O52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q52" s="2">
         <v>0</v>
@@ -4527,7 +4527,7 @@
         <v>0</v>
       </c>
       <c r="U52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:21" s="2" customFormat="1">
@@ -4577,19 +4577,19 @@
         <v>0</v>
       </c>
       <c r="P53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U53" s="2">
         <v>1</v>
@@ -4645,10 +4645,10 @@
         <v>0</v>
       </c>
       <c r="Q54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S54" s="2">
         <v>0</v>
@@ -4707,16 +4707,16 @@
         <v>0</v>
       </c>
       <c r="Q55" s="2">
+        <v>0</v>
+      </c>
+      <c r="R55" s="2">
         <v>2</v>
       </c>
-      <c r="R55" s="2">
-        <v>0</v>
-      </c>
       <c r="S55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U55" s="2">
         <v>0</v>
@@ -4775,10 +4775,10 @@
         <v>0</v>
       </c>
       <c r="R56" s="2">
+        <v>0</v>
+      </c>
+      <c r="S56" s="2">
         <v>5</v>
-      </c>
-      <c r="S56" s="2">
-        <v>0</v>
       </c>
       <c r="T56" s="2">
         <v>0</v>
@@ -4843,10 +4843,10 @@
         <v>0</v>
       </c>
       <c r="S57" s="2">
+        <v>0</v>
+      </c>
+      <c r="T57" s="2">
         <v>2</v>
-      </c>
-      <c r="T57" s="2">
-        <v>0</v>
       </c>
       <c r="U57" s="2">
         <v>0</v>
@@ -4908,10 +4908,10 @@
         <v>0</v>
       </c>
       <c r="T58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:21" s="2" customFormat="1">

</xml_diff>